<commit_message>
Implemented Features (Independent Test Case Execution, Comprehensive Message Capture, Expected Result Inclusion, Single Test Report Compilation)
Each test case initiates a fresh browser session, ensuring that the tests are independent of each other. This is crucial for accurate and reliable testing.
The code now captures all messages from the chatbot, including those contained within buttons. This ensures that all aspects of the chatbot’s responses are considered during testing.
A new column for ‘Expected Result’ has been added to the test report. This allows for a direct comparison between the expected and actual results, making it easier to identify discrepancies.
Despite each test case being independent, all results are collated into a single test report. This provides a comprehensive overview of the testing process and outcomes.
</commit_message>
<xml_diff>
--- a/resources/TestData.xlsx
+++ b/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivona\qa-rba-master\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDB4E1A-28B7-4304-BFA1-F6CAA105D1B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60A3EFD-1E15-482B-B2B4-5F9EFE13891E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -61,10 +61,24 @@
     <t>Dobra večer</t>
   </si>
   <si>
-    <t>Ok, samo polako jer još učim.</t>
-  </si>
-  <si>
     <t>PROMPT</t>
+  </si>
+  <si>
+    <t>Dobar dan! ☀️ Kako vam mogu pomoći?</t>
+  </si>
+  <si>
+    <t>kartice</t>
+  </si>
+  <si>
+    <t>HR523</t>
+  </si>
+  <si>
+    <t>Kod nas možete ugovoriti dvije vrsta kartica ovisno o tome što vam treba.
+Debitne kartice koje su vezane uz tekući, žiro, zaštićeni ili multivalutni tekući račun. Kada plaćate debitnim karticama, novac se odmah skida s računa.
+Kreditne kartice kod kojih ne plaćate kupnju odmah, nego kasnije.
+Koje vas kartice zanimaju?
+Debitne kartice
+Kreditne kartice</t>
   </si>
 </sst>
 </file>
@@ -391,16 +405,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -408,7 +422,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -422,10 +436,10 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -436,7 +450,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -445,6 +459,17 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved Chatbot Testing Accuracy
This commit includes updates to improve the accuracy of the test results. Changes include standardizing spaces before comparison, ignoring messages sent by the chatbot before the prompt, and removing specific unwanted text from the received message.
</commit_message>
<xml_diff>
--- a/resources/TestData.xlsx
+++ b/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivona\qa-rba-master\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF72CDA-F307-408C-BBC1-943281E722E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E25C1E0-DD37-438D-B6E6-FD2FCC1196DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -59,6 +59,17 @@
 Koje vas kartice zanimaju?
 Debitne kartice
 Kreditne kartice</t>
+  </si>
+  <si>
+    <t>izvod</t>
+  </si>
+  <si>
+    <t>HR001</t>
+  </si>
+  <si>
+    <t>Za koju uslugu vas zanima izvadak?
+Za kreditnu karticu
+Tekući i drugi računi</t>
   </si>
 </sst>
 </file>
@@ -385,19 +396,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,25 +419,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhanced Error Handling and Debugging in Chatbot Testing
This commit introduces improved error handling by adding specific error messages to identify scenarios where the chatbot does not understand the user’s question. Debugging information is now printed throughout the code to aid in identifying issues and understanding the flow of data. The formatting of received messages and error messages has been standardized for accurate comparison. This enhancement aids in distinguishing between failed test cases and error scenarios, improving the overall testing process of the chatbot.
</commit_message>
<xml_diff>
--- a/resources/TestData.xlsx
+++ b/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivona\qa-rba-master\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E25C1E0-DD37-438D-B6E6-FD2FCC1196DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49435E6-79BF-414C-84A6-583311A5B3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -70,6 +70,21 @@
     <t>Za koju uslugu vas zanima izvadak?
 Za kreditnu karticu
 Tekući i drugi računi</t>
+  </si>
+  <si>
+    <t>hr000</t>
+  </si>
+  <si>
+    <t>gedrgr</t>
+  </si>
+  <si>
+    <t>hr265</t>
+  </si>
+  <si>
+    <t>hghjhj</t>
+  </si>
+  <si>
+    <t>ispričaj mi vic</t>
   </si>
 </sst>
 </file>
@@ -396,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,6 +467,28 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>265</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>